<commit_message>
Updated knowledgeScraper - Updated knowledgeParser - UpdatedknowledgeInheritor - Updated knowledgeFilter - Removed knowledgeParser_ - Removed LOVScraper_
</commit_message>
<xml_diff>
--- a/RapidMinerCode/knowledgeFilter/Predicate.xlsx
+++ b/RapidMinerCode/knowledgeFilter/Predicate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EA63B4-093F-4E97-9C54-9FCA2ACDB344}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C6173-0868-4D70-AC90-349FAF507CA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="690" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <t>domain</t>
   </si>
   <si>
-    <t>Predicate</t>
+    <t>PredicateTerm</t>
   </si>
 </sst>
 </file>

</xml_diff>